<commit_message>
start working on cie xyz spec
</commit_message>
<xml_diff>
--- a/asset/experimentResult/comparison.xlsx
+++ b/asset/experimentResult/comparison.xlsx
@@ -571,38 +571,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1811,11 +1780,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="897765152"/>
-        <c:axId val="897774400"/>
+        <c:axId val="663749472"/>
+        <c:axId val="663750016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="897765152"/>
+        <c:axId val="663749472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1919,7 +1888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="897774400"/>
+        <c:crossAx val="663750016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1927,7 +1896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="897774400"/>
+        <c:axId val="663750016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2039,7 +2008,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="897765152"/>
+        <c:crossAx val="663749472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2681,15 +2650,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>247651</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2977,7 +2946,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>